<commit_message>
Creating tables from the csvs within the ipynb file (2 out of 5)
</commit_message>
<xml_diff>
--- a/pre_processed_data/Analysis.xlsx
+++ b/pre_processed_data/Analysis.xlsx
@@ -431,7 +431,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,6 +441,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -507,7 +513,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -573,10 +579,12 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -585,8 +593,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Incorreto" xfId="2" builtinId="27"/>
@@ -871,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -918,10 +925,10 @@
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="67" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="67" t="s">
         <v>106</v>
       </c>
       <c r="P3" s="42" t="s">
@@ -1062,15 +1069,15 @@
       <c r="B6" s="47">
         <v>0.178651789044733</v>
       </c>
-      <c r="C6" s="65">
+      <c r="C6" s="61">
         <f>C40*$F$44</f>
         <v>-14.245749712799199</v>
       </c>
-      <c r="D6" s="65">
+      <c r="D6" s="61">
         <f t="shared" ref="D6:E6" si="0">D40*$F$44</f>
         <v>13.168131768538199</v>
       </c>
-      <c r="E6" s="65">
+      <c r="E6" s="61">
         <f t="shared" si="0"/>
         <v>15.056045822043101</v>
       </c>
@@ -1080,13 +1087,13 @@
       <c r="H6" s="47">
         <v>0.38306047475021598</v>
       </c>
-      <c r="I6" s="65">
+      <c r="I6" s="61">
         <v>-0.196287175937785</v>
       </c>
-      <c r="J6" s="65">
+      <c r="J6" s="61">
         <v>8.6866693559898012E-2</v>
       </c>
-      <c r="K6" s="65">
+      <c r="K6" s="61">
         <v>7.9569474126831019E-2</v>
       </c>
       <c r="P6" s="49" t="s">
@@ -1144,7 +1151,7 @@
         <v>21.938332447183701</v>
       </c>
       <c r="AL6" s="53">
-        <f>AI6/AJ6</f>
+        <f t="shared" ref="AL6:AL28" si="1">AI6/AJ6</f>
         <v>0.47807072402327611</v>
       </c>
     </row>
@@ -1155,16 +1162,16 @@
       <c r="B7" s="54">
         <v>1</v>
       </c>
-      <c r="C7" s="65">
-        <f t="shared" ref="C7:E7" si="1">C41*$F$44</f>
+      <c r="C7" s="61">
+        <f t="shared" ref="C7:E7" si="2">C41*$F$44</f>
         <v>-90.577729178057226</v>
       </c>
-      <c r="D7" s="65">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="65">
-        <f t="shared" si="1"/>
+      <c r="D7" s="61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="61">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G7" s="48" t="s">
@@ -1173,13 +1180,13 @@
       <c r="H7" s="47">
         <v>0</v>
       </c>
-      <c r="I7" s="65">
+      <c r="I7" s="61">
         <v>0.29213830538841501</v>
       </c>
-      <c r="J7" s="65">
-        <v>0</v>
-      </c>
-      <c r="K7" s="65">
+      <c r="J7" s="61">
+        <v>0</v>
+      </c>
+      <c r="K7" s="61">
         <v>0</v>
       </c>
       <c r="P7" s="48" t="s">
@@ -1237,7 +1244,7 @@
         <v>0.306834582623074</v>
       </c>
       <c r="AL7" s="53">
-        <f>AI7/AJ7</f>
+        <f t="shared" si="1"/>
         <v>12.770334355756233</v>
       </c>
     </row>
@@ -1248,16 +1255,16 @@
       <c r="B8" s="57">
         <v>0.298363636363636</v>
       </c>
-      <c r="C8" s="65">
-        <f t="shared" ref="C8:E8" si="2">C42*$F$44</f>
+      <c r="C8" s="61">
+        <f t="shared" ref="C8:E8" si="3">C42*$F$44</f>
         <v>-1.1345195611400016</v>
       </c>
-      <c r="D8" s="65">
-        <f t="shared" si="2"/>
+      <c r="D8" s="61">
+        <f t="shared" si="3"/>
         <v>-0.89797671342489727</v>
       </c>
-      <c r="E8" s="65">
-        <f t="shared" si="2"/>
+      <c r="E8" s="61">
+        <f t="shared" si="3"/>
         <v>7.2351713859910021</v>
       </c>
       <c r="G8" s="44" t="s">
@@ -1266,13 +1273,13 @@
       <c r="H8" s="57">
         <v>0.27123574578583098</v>
       </c>
-      <c r="I8" s="65">
+      <c r="I8" s="61">
         <v>-0.27123574578583098</v>
       </c>
-      <c r="J8" s="65">
+      <c r="J8" s="61">
         <v>0.188344141661968</v>
       </c>
-      <c r="K8" s="65">
+      <c r="K8" s="61">
         <v>0.17335559136934603</v>
       </c>
       <c r="P8" s="44" t="s">
@@ -1330,7 +1337,7 @@
         <v>0.27035655885081</v>
       </c>
       <c r="AL8" s="53">
-        <f>AI8/AJ8</f>
+        <f t="shared" si="1"/>
         <v>2.5537083623046417</v>
       </c>
     </row>
@@ -1341,16 +1348,16 @@
       <c r="B9" s="47">
         <v>0.19426289034132099</v>
       </c>
-      <c r="C9" s="65">
-        <f t="shared" ref="C9:E9" si="3">C43*$F$44</f>
+      <c r="C9" s="61">
+        <f t="shared" ref="C9:E9" si="4">C43*$F$44</f>
         <v>-14.252916143347749</v>
       </c>
-      <c r="D9" s="65">
-        <f t="shared" si="3"/>
+      <c r="D9" s="61">
+        <f t="shared" si="4"/>
         <v>7.6711958199159991</v>
       </c>
-      <c r="E9" s="65">
-        <f t="shared" si="3"/>
+      <c r="E9" s="61">
+        <f t="shared" si="4"/>
         <v>8.9158559809736033</v>
       </c>
       <c r="G9" s="48" t="s">
@@ -1359,13 +1366,13 @@
       <c r="H9" s="47">
         <v>0</v>
       </c>
-      <c r="I9" s="65">
-        <v>0</v>
-      </c>
-      <c r="J9" s="65">
-        <v>0</v>
-      </c>
-      <c r="K9" s="65">
+      <c r="I9" s="61">
+        <v>0</v>
+      </c>
+      <c r="J9" s="61">
+        <v>0</v>
+      </c>
+      <c r="K9" s="61">
         <v>0</v>
       </c>
       <c r="P9" s="48" t="s">
@@ -1423,7 +1430,7 @@
         <v>0.24715358979390201</v>
       </c>
       <c r="AL9" s="53">
-        <f>AI9/AJ9</f>
+        <f t="shared" si="1"/>
         <v>14.013803276795935</v>
       </c>
     </row>
@@ -1434,16 +1441,16 @@
       <c r="B10" s="47">
         <v>0.18634926538962199</v>
       </c>
-      <c r="C10" s="65">
-        <f t="shared" ref="C10:E10" si="4">C44*$F$44</f>
+      <c r="C10" s="61">
+        <f t="shared" ref="C10:E10" si="5">C44*$F$44</f>
         <v>-15.0286707891922</v>
       </c>
-      <c r="D10" s="65">
-        <f t="shared" si="4"/>
+      <c r="D10" s="61">
+        <f t="shared" si="5"/>
         <v>10.012794231589</v>
       </c>
-      <c r="E10" s="65">
-        <f t="shared" si="4"/>
+      <c r="E10" s="61">
+        <f t="shared" si="5"/>
         <v>8.9084524564714993</v>
       </c>
       <c r="G10" s="48" t="s">
@@ -1452,13 +1459,13 @@
       <c r="H10" s="47">
         <v>9.6317050668594403E-2</v>
       </c>
-      <c r="I10" s="65">
+      <c r="I10" s="61">
         <v>-9.6317050668594403E-2</v>
       </c>
-      <c r="J10" s="65">
+      <c r="J10" s="61">
         <v>2.63733863029606E-2</v>
       </c>
-      <c r="K10" s="65">
+      <c r="K10" s="61">
         <v>0.38219992137739156</v>
       </c>
       <c r="P10" s="49" t="s">
@@ -1516,7 +1523,7 @@
         <v>0.21263930158212999</v>
       </c>
       <c r="AL10" s="53">
-        <f>AI10/AJ10</f>
+        <f t="shared" si="1"/>
         <v>5.8353094155313014</v>
       </c>
     </row>
@@ -1527,16 +1534,16 @@
       <c r="B11" s="47">
         <v>0.18465703971119099</v>
       </c>
-      <c r="C11" s="65">
-        <f t="shared" ref="C11:E11" si="5">C45*$F$44</f>
+      <c r="C11" s="61">
+        <f t="shared" ref="C11:E11" si="6">C45*$F$44</f>
         <v>-14.77634776377729</v>
       </c>
-      <c r="D11" s="65">
-        <f t="shared" si="5"/>
+      <c r="D11" s="61">
+        <f t="shared" si="6"/>
         <v>10.110985404686398</v>
       </c>
-      <c r="E11" s="65">
-        <f t="shared" si="5"/>
+      <c r="E11" s="61">
+        <f t="shared" si="6"/>
         <v>8.9728663937356981</v>
       </c>
       <c r="G11" s="48" t="s">
@@ -1545,13 +1552,13 @@
       <c r="H11" s="47">
         <v>0.38938825955384898</v>
       </c>
-      <c r="I11" s="65">
+      <c r="I11" s="61">
         <v>-0.20294242440479998</v>
       </c>
-      <c r="J11" s="65">
+      <c r="J11" s="61">
         <v>5.7344342016420025E-2</v>
       </c>
-      <c r="K11" s="65">
+      <c r="K11" s="61">
         <v>6.2726789046359033E-2</v>
       </c>
       <c r="P11" s="44" t="s">
@@ -1609,7 +1616,7 @@
         <v>0.19330669309749801</v>
       </c>
       <c r="AL11" s="53">
-        <f>AI11/AJ11</f>
+        <f t="shared" si="1"/>
         <v>7.8107296074145447</v>
       </c>
     </row>
@@ -1620,16 +1627,16 @@
       <c r="B12" s="47">
         <v>0.18433179723502299</v>
       </c>
-      <c r="C12" s="65">
-        <f t="shared" ref="C12:E12" si="6">C46*$F$44</f>
+      <c r="C12" s="61">
+        <f t="shared" ref="C12:E12" si="7">C46*$F$44</f>
         <v>-15.067252683261609</v>
       </c>
-      <c r="D12" s="65">
-        <f t="shared" si="6"/>
+      <c r="D12" s="61">
+        <f t="shared" si="7"/>
         <v>9.8349148112096021</v>
       </c>
-      <c r="E12" s="65">
-        <f t="shared" si="6"/>
+      <c r="E12" s="61">
+        <f t="shared" si="7"/>
         <v>9.825691392511601</v>
       </c>
       <c r="G12" s="48" t="s">
@@ -1638,13 +1645,13 @@
       <c r="H12" s="47">
         <v>0.38075566920947101</v>
       </c>
-      <c r="I12" s="65">
+      <c r="I12" s="61">
         <v>-0.21923616978840801</v>
       </c>
-      <c r="J12" s="65">
+      <c r="J12" s="61">
         <v>6.7253896948391012E-2</v>
       </c>
-      <c r="K12" s="65">
+      <c r="K12" s="61">
         <v>6.9632428970497984E-2</v>
       </c>
       <c r="P12" s="48" t="s">
@@ -1702,7 +1709,7 @@
         <v>0.140012445274206</v>
       </c>
       <c r="AL12" s="53">
-        <f>AI12/AJ12</f>
+        <f t="shared" si="1"/>
         <v>2.7142229218981111</v>
       </c>
     </row>
@@ -1713,16 +1720,16 @@
       <c r="B13" s="47">
         <v>0.18144252441773101</v>
       </c>
-      <c r="C13" s="65">
-        <f t="shared" ref="C13:E13" si="7">C47*$F$44</f>
+      <c r="C13" s="61">
+        <f t="shared" ref="C13:E13" si="8">C47*$F$44</f>
         <v>-14.331168329623573</v>
       </c>
-      <c r="D13" s="65">
-        <f t="shared" si="7"/>
+      <c r="D13" s="61">
+        <f t="shared" si="8"/>
         <v>10.1576343506797</v>
       </c>
-      <c r="E13" s="65">
-        <f t="shared" si="7"/>
+      <c r="E13" s="61">
+        <f t="shared" si="8"/>
         <v>10.8572159870081</v>
       </c>
       <c r="G13" s="48" t="s">
@@ -1731,13 +1738,13 @@
       <c r="H13" s="47">
         <v>0.38316128344292499</v>
       </c>
-      <c r="I13" s="65">
+      <c r="I13" s="61">
         <v>-0.21308274336882599</v>
       </c>
-      <c r="J13" s="65">
+      <c r="J13" s="61">
         <v>6.0586813014464003E-2</v>
       </c>
-      <c r="K13" s="65">
+      <c r="K13" s="61">
         <v>6.6657965783244011E-2</v>
       </c>
       <c r="P13" s="49" t="s">
@@ -1795,7 +1802,7 @@
         <v>9.2064908381742E-2</v>
       </c>
       <c r="AL13" s="53">
-        <f>AI13/AJ13</f>
+        <f t="shared" si="1"/>
         <v>2.4118267082207033E-13</v>
       </c>
     </row>
@@ -1806,16 +1813,16 @@
       <c r="B14" s="57">
         <v>0.1787719955073</v>
       </c>
-      <c r="C14" s="65">
-        <f t="shared" ref="C14:E14" si="8">C48*$F$44</f>
+      <c r="C14" s="61">
+        <f t="shared" ref="C14:E14" si="9">C48*$F$44</f>
         <v>-14.895631065005391</v>
       </c>
-      <c r="D14" s="65">
-        <f t="shared" si="8"/>
+      <c r="D14" s="61">
+        <f t="shared" si="9"/>
         <v>10.291024748335397</v>
       </c>
-      <c r="E14" s="65">
-        <f t="shared" si="8"/>
+      <c r="E14" s="61">
+        <f t="shared" si="9"/>
         <v>9.0820480981728018</v>
       </c>
       <c r="G14" s="44" t="s">
@@ -1824,13 +1831,13 @@
       <c r="H14" s="57">
         <v>0.346875499467236</v>
       </c>
-      <c r="I14" s="65">
+      <c r="I14" s="61">
         <v>-0.23797679092034801</v>
       </c>
-      <c r="J14" s="65">
+      <c r="J14" s="61">
         <v>0.10149330858049699</v>
       </c>
-      <c r="K14" s="65">
+      <c r="K14" s="61">
         <v>0.10331607642096402</v>
       </c>
       <c r="P14" s="44" t="s">
@@ -1888,7 +1895,7 @@
         <v>5.4600983178325097E-2</v>
       </c>
       <c r="AL14" s="53">
-        <f>AI14/AJ14</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1899,16 +1906,16 @@
       <c r="B15" s="47">
         <v>0.175924205833178</v>
       </c>
-      <c r="C15" s="65">
-        <f t="shared" ref="C15:E15" si="9">C49*$F$44</f>
+      <c r="C15" s="61">
+        <f t="shared" ref="C15:E15" si="10">C49*$F$44</f>
         <v>-14.911703260337589</v>
       </c>
-      <c r="D15" s="65">
-        <f t="shared" si="9"/>
+      <c r="D15" s="61">
+        <f t="shared" si="10"/>
         <v>10.693399483324098</v>
       </c>
-      <c r="E15" s="65">
-        <f t="shared" si="9"/>
+      <c r="E15" s="61">
+        <f t="shared" si="10"/>
         <v>10.206807215909999</v>
       </c>
       <c r="G15" s="48" t="s">
@@ -1917,13 +1924,13 @@
       <c r="H15" s="47">
         <v>0.37113573208225797</v>
       </c>
-      <c r="I15" s="65">
+      <c r="I15" s="61">
         <v>-0.23088341372159998</v>
       </c>
-      <c r="J15" s="65">
+      <c r="J15" s="61">
         <v>8.2740344077188999E-2</v>
       </c>
-      <c r="K15" s="65">
+      <c r="K15" s="61">
         <v>8.2972158837631038E-2</v>
       </c>
       <c r="P15" s="44" t="s">
@@ -1981,7 +1988,7 @@
         <v>1.9483850263166801E-2</v>
       </c>
       <c r="AL15" s="53">
-        <f>AI15/AJ15</f>
+        <f t="shared" si="1"/>
         <v>8.053414421066872E-10</v>
       </c>
     </row>
@@ -1992,16 +1999,16 @@
       <c r="B16" s="47">
         <v>0.175720014582573</v>
       </c>
-      <c r="C16" s="65">
-        <f t="shared" ref="C16:E16" si="10">C50*$F$44</f>
+      <c r="C16" s="61">
+        <f t="shared" ref="C16:E16" si="11">C50*$F$44</f>
         <v>-13.624149824030349</v>
       </c>
-      <c r="D16" s="65">
-        <f t="shared" si="10"/>
+      <c r="D16" s="61">
+        <f t="shared" si="11"/>
         <v>10.7305748253166</v>
       </c>
-      <c r="E16" s="65">
-        <f t="shared" si="10"/>
+      <c r="E16" s="61">
+        <f t="shared" si="11"/>
         <v>10.387182215212002</v>
       </c>
       <c r="G16" s="48" t="s">
@@ -2010,13 +2017,13 @@
       <c r="H16" s="47">
         <v>0.37752758699532601</v>
       </c>
-      <c r="I16" s="65">
+      <c r="I16" s="61">
         <v>-0.21810039164345901</v>
       </c>
-      <c r="J16" s="65">
+      <c r="J16" s="61">
         <v>7.4189394537323983E-2</v>
       </c>
-      <c r="K16" s="65">
+      <c r="K16" s="61">
         <v>7.3814661778266011E-2</v>
       </c>
       <c r="P16" s="48" t="s">
@@ -2074,7 +2081,7 @@
         <v>1.0203975964810199E-2</v>
       </c>
       <c r="AL16" s="53">
-        <f>AI16/AJ16</f>
+        <f t="shared" si="1"/>
         <v>2.1760596623345543E-12</v>
       </c>
     </row>
@@ -2085,16 +2092,16 @@
       <c r="B17" s="47">
         <v>0.175627240143369</v>
       </c>
-      <c r="C17" s="65">
-        <f t="shared" ref="C17:E17" si="11">C51*$F$44</f>
+      <c r="C17" s="61">
+        <f t="shared" ref="C17:E17" si="12">C51*$F$44</f>
         <v>-14.454294685391941</v>
       </c>
-      <c r="D17" s="65">
-        <f t="shared" si="11"/>
+      <c r="D17" s="61">
+        <f t="shared" si="12"/>
         <v>11.137570536473101</v>
       </c>
-      <c r="E17" s="65">
-        <f t="shared" si="11"/>
+      <c r="E17" s="61">
+        <f t="shared" si="12"/>
         <v>10.5933586176447</v>
       </c>
       <c r="G17" s="48" t="s">
@@ -2103,13 +2110,13 @@
       <c r="H17" s="47">
         <v>0.38801909411303598</v>
       </c>
-      <c r="I17" s="65">
+      <c r="I17" s="61">
         <v>-0.19951862421720198</v>
       </c>
-      <c r="J17" s="65">
+      <c r="J17" s="61">
         <v>5.818510721391601E-2</v>
       </c>
-      <c r="K17" s="65">
+      <c r="K17" s="61">
         <v>6.3759807773653032E-2</v>
       </c>
       <c r="Y17" s="44" t="s">
@@ -2146,7 +2153,7 @@
         <v>9.5315497949181194E-3</v>
       </c>
       <c r="AL17" s="53">
-        <f>AI17/AJ17</f>
+        <f t="shared" si="1"/>
         <v>0.87433227823006043</v>
       </c>
     </row>
@@ -2157,16 +2164,16 @@
       <c r="B18" s="47">
         <v>0.175390266299357</v>
       </c>
-      <c r="C18" s="65">
-        <f t="shared" ref="C18:E18" si="12">C52*$F$44</f>
+      <c r="C18" s="61">
+        <f t="shared" ref="C18:E18" si="13">C52*$F$44</f>
         <v>-14.2111488339728</v>
       </c>
-      <c r="D18" s="65">
-        <f t="shared" si="12"/>
+      <c r="D18" s="61">
+        <f t="shared" si="13"/>
         <v>10.547562986648401</v>
       </c>
-      <c r="E18" s="65">
-        <f t="shared" si="12"/>
+      <c r="E18" s="61">
+        <f t="shared" si="13"/>
         <v>9.5929009684967976</v>
       </c>
       <c r="G18" s="48" t="s">
@@ -2175,13 +2182,13 @@
       <c r="H18" s="47">
         <v>0.39563217737890399</v>
       </c>
-      <c r="I18" s="65">
+      <c r="I18" s="61">
         <v>-0.17414323814910998</v>
       </c>
-      <c r="J18" s="65">
+      <c r="J18" s="61">
         <v>5.502704170503403E-2</v>
       </c>
-      <c r="K18" s="65">
+      <c r="K18" s="61">
         <v>4.883095944904603E-2</v>
       </c>
       <c r="Y18" s="44" t="s">
@@ -2218,7 +2225,7 @@
         <v>-6.0195401671708199E-2</v>
       </c>
       <c r="AL18" s="53">
-        <f>AI18/AJ18</f>
+        <f t="shared" si="1"/>
         <v>-3.6961342612918631</v>
       </c>
     </row>
@@ -2229,16 +2236,16 @@
       <c r="B19" s="47">
         <v>0.172969966629588</v>
       </c>
-      <c r="C19" s="65">
-        <f t="shared" ref="C19:E19" si="13">C53*$F$44</f>
+      <c r="C19" s="61">
+        <f t="shared" ref="C19:E19" si="14">C53*$F$44</f>
         <v>-14.580901966684259</v>
       </c>
-      <c r="D19" s="65">
-        <f t="shared" si="13"/>
+      <c r="D19" s="61">
+        <f t="shared" si="14"/>
         <v>11.942233401202499</v>
       </c>
-      <c r="E19" s="65">
-        <f t="shared" si="13"/>
+      <c r="E19" s="61">
+        <f t="shared" si="14"/>
         <v>11.139984329844301</v>
       </c>
       <c r="G19" s="48" t="s">
@@ -2247,13 +2254,13 @@
       <c r="H19" s="47">
         <v>0.35271069784695602</v>
       </c>
-      <c r="I19" s="65">
+      <c r="I19" s="61">
         <v>-0.20711405123085602</v>
       </c>
-      <c r="J19" s="65">
+      <c r="J19" s="61">
         <v>0.10582432957636095</v>
       </c>
-      <c r="K19" s="65">
+      <c r="K19" s="61">
         <v>9.8553590938120994E-2</v>
       </c>
       <c r="P19" s="42" t="s">
@@ -2293,7 +2300,7 @@
         <v>-0.15607014742570099</v>
       </c>
       <c r="AL19" s="53">
-        <f>AI19/AJ19</f>
+        <f t="shared" si="1"/>
         <v>1.4912662584345546</v>
       </c>
     </row>
@@ -2304,16 +2311,16 @@
       <c r="B20" s="47">
         <v>0.17216937138593499</v>
       </c>
-      <c r="C20" s="65">
-        <f t="shared" ref="C20:E20" si="14">C54*$F$44</f>
+      <c r="C20" s="61">
+        <f t="shared" ref="C20:E20" si="15">C54*$F$44</f>
         <v>-14.607122766235481</v>
       </c>
-      <c r="D20" s="65">
-        <f t="shared" si="14"/>
+      <c r="D20" s="61">
+        <f t="shared" si="15"/>
         <v>11.267911346254902</v>
       </c>
-      <c r="E20" s="65">
-        <f t="shared" si="14"/>
+      <c r="E20" s="61">
+        <f t="shared" si="15"/>
         <v>11.346699225042803</v>
       </c>
       <c r="G20" s="48" t="s">
@@ -2322,13 +2329,13 @@
       <c r="H20" s="47">
         <v>0.373643348384816</v>
       </c>
-      <c r="I20" s="65">
+      <c r="I20" s="61">
         <v>-0.19912830317577701</v>
       </c>
-      <c r="J20" s="65">
+      <c r="J20" s="61">
         <v>7.6587968056676003E-2</v>
       </c>
-      <c r="K20" s="65">
+      <c r="K20" s="61">
         <v>7.8863117793832982E-2</v>
       </c>
       <c r="Y20" s="44" t="s">
@@ -2365,7 +2372,7 @@
         <v>-0.32352987354530799</v>
       </c>
       <c r="AL20" s="53">
-        <f>AI20/AJ20</f>
+        <f t="shared" si="1"/>
         <v>1.58451003861183</v>
       </c>
     </row>
@@ -2376,16 +2383,16 @@
       <c r="B21" s="47">
         <v>0.17214771265845999</v>
       </c>
-      <c r="C21" s="65">
-        <f t="shared" ref="C21:E21" si="15">C55*$F$44</f>
+      <c r="C21" s="61">
+        <f t="shared" ref="C21:E21" si="16">C55*$F$44</f>
         <v>-14.787133544090638</v>
       </c>
-      <c r="D21" s="65">
-        <f t="shared" si="15"/>
+      <c r="D21" s="61">
+        <f t="shared" si="16"/>
         <v>10.603543217919</v>
       </c>
-      <c r="E21" s="65">
-        <f t="shared" si="15"/>
+      <c r="E21" s="61">
+        <f t="shared" si="16"/>
         <v>11.055034414273498</v>
       </c>
       <c r="G21" s="48" t="s">
@@ -2394,13 +2401,13 @@
       <c r="H21" s="47">
         <v>0.38775454318824898</v>
       </c>
-      <c r="I21" s="65">
+      <c r="I21" s="61">
         <v>-0.20740398477939298</v>
       </c>
-      <c r="J21" s="65">
+      <c r="J21" s="61">
         <v>6.2503528904828021E-2</v>
       </c>
-      <c r="K21" s="65">
+      <c r="K21" s="61">
         <v>6.2548053389641034E-2</v>
       </c>
       <c r="Y21" s="44" t="s">
@@ -2437,7 +2444,7 @@
         <v>-0.48129109173703499</v>
       </c>
       <c r="AL21" s="53">
-        <f>AI21/AJ21</f>
+        <f t="shared" si="1"/>
         <v>6.7099902764896973</v>
       </c>
     </row>
@@ -2448,16 +2455,16 @@
       <c r="B22" s="47">
         <v>0.17182067703568099</v>
       </c>
-      <c r="C22" s="65">
-        <f t="shared" ref="C22:E22" si="16">C56*$F$44</f>
+      <c r="C22" s="61">
+        <f t="shared" ref="C22:E22" si="17">C56*$F$44</f>
         <v>-14.972425629061171</v>
       </c>
-      <c r="D22" s="65">
-        <f t="shared" si="16"/>
+      <c r="D22" s="61">
+        <f t="shared" si="17"/>
         <v>11.861253596070803</v>
       </c>
-      <c r="E22" s="65">
-        <f t="shared" si="16"/>
+      <c r="E22" s="61">
+        <f t="shared" si="17"/>
         <v>10.986437087608902</v>
       </c>
       <c r="G22" s="48" t="s">
@@ -2466,13 +2473,13 @@
       <c r="H22" s="47">
         <v>0.378221307270945</v>
       </c>
-      <c r="I22" s="65">
+      <c r="I22" s="61">
         <v>-0.21566906975071701</v>
       </c>
-      <c r="J22" s="65">
+      <c r="J22" s="61">
         <v>7.2892449036184026E-2</v>
       </c>
-      <c r="K22" s="65">
+      <c r="K22" s="61">
         <v>7.6640257567313019E-2</v>
       </c>
       <c r="Y22" s="44" t="s">
@@ -2509,7 +2516,7 @@
         <v>-0.56621490664862906</v>
       </c>
       <c r="AL22" s="53">
-        <f>AI22/AJ22</f>
+        <f t="shared" si="1"/>
         <v>4.8374294662455632</v>
       </c>
     </row>
@@ -2520,16 +2527,16 @@
       <c r="B23" s="57">
         <v>0.170228863249479</v>
       </c>
-      <c r="C23" s="65">
-        <f t="shared" ref="C23:E23" si="17">C57*$F$44</f>
+      <c r="C23" s="61">
+        <f t="shared" ref="C23:E23" si="18">C57*$F$44</f>
         <v>-14.624630510994418</v>
       </c>
-      <c r="D23" s="65">
-        <f t="shared" si="17"/>
+      <c r="D23" s="61">
+        <f t="shared" si="18"/>
         <v>11.644873835431103</v>
       </c>
-      <c r="E23" s="65">
-        <f t="shared" si="17"/>
+      <c r="E23" s="61">
+        <f t="shared" si="18"/>
         <v>10.6859486444908</v>
       </c>
       <c r="G23" s="44" t="s">
@@ -2538,13 +2545,13 @@
       <c r="H23" s="57">
         <v>0.38538439868611202</v>
       </c>
-      <c r="I23" s="65">
+      <c r="I23" s="61">
         <v>-0.19387231009413403</v>
       </c>
-      <c r="J23" s="65">
+      <c r="J23" s="61">
         <v>6.8384449060448993E-2</v>
       </c>
-      <c r="K23" s="65">
+      <c r="K23" s="61">
         <v>6.5081125325722966E-2</v>
       </c>
       <c r="Y23" s="44" t="s">
@@ -2581,7 +2588,7 @@
         <v>-0.57024146928462305</v>
       </c>
       <c r="AL23" s="53">
-        <f>AI23/AJ23</f>
+        <f t="shared" si="1"/>
         <v>1.3445712725277066</v>
       </c>
     </row>
@@ -2592,16 +2599,16 @@
       <c r="B24" s="47">
         <v>0.16774911857487401</v>
       </c>
-      <c r="C24" s="65">
-        <f t="shared" ref="C24:E24" si="18">C58*$F$44</f>
+      <c r="C24" s="61">
+        <f t="shared" ref="C24:E24" si="19">C58*$F$44</f>
         <v>-13.630487725860352</v>
       </c>
-      <c r="D24" s="65">
-        <f t="shared" si="18"/>
+      <c r="D24" s="61">
+        <f t="shared" si="19"/>
         <v>11.955885509008501</v>
       </c>
-      <c r="E24" s="65">
-        <f t="shared" si="18"/>
+      <c r="E24" s="61">
+        <f t="shared" si="19"/>
         <v>11.478419042311799</v>
       </c>
       <c r="G24" s="48" t="s">
@@ -2610,13 +2617,13 @@
       <c r="H24" s="47">
         <v>0.377508778288555</v>
       </c>
-      <c r="I24" s="65">
+      <c r="I24" s="61">
         <v>-0.22360285011570299</v>
       </c>
-      <c r="J24" s="65">
+      <c r="J24" s="61">
         <v>7.2802075991046988E-2</v>
       </c>
-      <c r="K24" s="65">
+      <c r="K24" s="61">
         <v>7.059531984700701E-2</v>
       </c>
       <c r="Y24" s="44" t="s">
@@ -2653,7 +2660,7 @@
         <v>-2.3923386630591299</v>
       </c>
       <c r="AL24" s="53">
-        <f>AI24/AJ24</f>
+        <f t="shared" si="1"/>
         <v>1.9031736558484371</v>
       </c>
     </row>
@@ -2664,16 +2671,16 @@
       <c r="B25" s="47">
         <v>0.164950349393159</v>
       </c>
-      <c r="C25" s="65">
-        <f t="shared" ref="C25:E25" si="19">C59*$F$44</f>
+      <c r="C25" s="61">
+        <f t="shared" ref="C25:E25" si="20">C59*$F$44</f>
         <v>-14.487668456811301</v>
       </c>
-      <c r="D25" s="65">
-        <f t="shared" si="19"/>
+      <c r="D25" s="61">
+        <f t="shared" si="20"/>
         <v>12.579854928525503</v>
       </c>
-      <c r="E25" s="65">
-        <f t="shared" si="19"/>
+      <c r="E25" s="61">
+        <f t="shared" si="20"/>
         <v>12.529620608182201</v>
       </c>
       <c r="G25" s="48" t="s">
@@ -2682,13 +2689,13 @@
       <c r="H25" s="47">
         <v>0.20986563660865201</v>
       </c>
-      <c r="I25" s="65">
+      <c r="I25" s="61">
         <v>-0.17104719143410391</v>
       </c>
-      <c r="J25" s="65">
+      <c r="J25" s="61">
         <v>0.181302990226445</v>
       </c>
-      <c r="K25" s="65">
+      <c r="K25" s="61">
         <v>0.17535861574689196</v>
       </c>
       <c r="Y25" s="44" t="s">
@@ -2725,7 +2732,7 @@
         <v>-3.16757051238028</v>
       </c>
       <c r="AL25" s="53">
-        <f>AI25/AJ25</f>
+        <f t="shared" si="1"/>
         <v>1.9729537072017225</v>
       </c>
     </row>
@@ -2736,16 +2743,16 @@
       <c r="B26" s="47">
         <v>0.16210758215531401</v>
       </c>
-      <c r="C26" s="65">
-        <f t="shared" ref="C26:E26" si="20">C60*$F$44</f>
+      <c r="C26" s="61">
+        <f t="shared" ref="C26:E26" si="21">C60*$F$44</f>
         <v>-14.340041416124111</v>
       </c>
-      <c r="D26" s="65">
-        <f t="shared" si="20"/>
+      <c r="D26" s="61">
+        <f t="shared" si="21"/>
         <v>12.149335596483702</v>
       </c>
-      <c r="E26" s="65">
-        <f t="shared" si="20"/>
+      <c r="E26" s="61">
+        <f t="shared" si="21"/>
         <v>12.151232734694799</v>
       </c>
       <c r="G26" s="48" t="s">
@@ -2754,13 +2761,13 @@
       <c r="H26" s="47">
         <v>0.375833736333341</v>
       </c>
-      <c r="I26" s="65">
+      <c r="I26" s="61">
         <v>-0.22283898137546698</v>
       </c>
-      <c r="J26" s="65">
+      <c r="J26" s="61">
         <v>7.1726758078354991E-2</v>
       </c>
-      <c r="K26" s="65">
+      <c r="K26" s="61">
         <v>7.6375899059904995E-2</v>
       </c>
       <c r="Y26" s="44" t="s">
@@ -2797,7 +2804,7 @@
         <v>-4.4437239908506001</v>
       </c>
       <c r="AL26" s="53">
-        <f>AI26/AJ26</f>
+        <f t="shared" si="1"/>
         <v>3.806626194225466</v>
       </c>
     </row>
@@ -2808,16 +2815,16 @@
       <c r="B27" s="47">
         <v>0.15734720416124801</v>
       </c>
-      <c r="C27" s="65">
-        <f t="shared" ref="C27:E27" si="21">C61*$F$44</f>
+      <c r="C27" s="61">
+        <f t="shared" ref="C27:E27" si="22">C61*$F$44</f>
         <v>-13.541737959984451</v>
       </c>
-      <c r="D27" s="65">
-        <f t="shared" si="21"/>
+      <c r="D27" s="61">
+        <f t="shared" si="22"/>
         <v>13.217976068322098</v>
       </c>
-      <c r="E27" s="65">
-        <f t="shared" si="21"/>
+      <c r="E27" s="61">
+        <f t="shared" si="22"/>
         <v>11.601685113829099</v>
       </c>
       <c r="G27" s="48" t="s">
@@ -2826,13 +2833,13 @@
       <c r="H27" s="47">
         <v>0.35745037140067198</v>
       </c>
-      <c r="I27" s="65">
+      <c r="I27" s="61">
         <v>-0.25630462049192498</v>
       </c>
-      <c r="J27" s="65">
+      <c r="J27" s="61">
         <v>9.4740172553331004E-2</v>
       </c>
-      <c r="K27" s="65">
+      <c r="K27" s="61">
         <v>9.5719793619731042E-2</v>
       </c>
       <c r="Y27" s="44" t="s">
@@ -2869,7 +2876,7 @@
         <v>-4.5386114853675501</v>
       </c>
       <c r="AL27" s="53">
-        <f>AI27/AJ27</f>
+        <f t="shared" si="1"/>
         <v>33.513083877926761</v>
       </c>
     </row>
@@ -2880,16 +2887,16 @@
       <c r="B28" s="47">
         <v>0.15038702543309901</v>
       </c>
-      <c r="C28" s="65">
-        <f t="shared" ref="C28:E28" si="22">C62*$F$44</f>
+      <c r="C28" s="61">
+        <f t="shared" ref="C28:E28" si="23">C62*$F$44</f>
         <v>-14.004970225573231</v>
       </c>
-      <c r="D28" s="65">
-        <f t="shared" si="22"/>
+      <c r="D28" s="61">
+        <f t="shared" si="23"/>
         <v>13.833874155353698</v>
       </c>
-      <c r="E28" s="65">
-        <f t="shared" si="22"/>
+      <c r="E28" s="61">
+        <f t="shared" si="23"/>
         <v>13.625011004124499</v>
       </c>
       <c r="G28" s="48" t="s">
@@ -2898,13 +2905,13 @@
       <c r="H28" s="47">
         <v>0.36412780929760302</v>
       </c>
-      <c r="I28" s="65">
+      <c r="I28" s="61">
         <v>-0.21767335441107602</v>
       </c>
-      <c r="J28" s="65">
+      <c r="J28" s="61">
         <v>8.1558345490408968E-2</v>
       </c>
-      <c r="K28" s="65">
+      <c r="K28" s="61">
         <v>8.9415023820063E-2</v>
       </c>
       <c r="Y28" s="44" t="s">
@@ -2941,7 +2948,7 @@
         <v>-4.60853937492322</v>
       </c>
       <c r="AL28" s="53">
-        <f>AI28/AJ28</f>
+        <f t="shared" si="1"/>
         <v>4.7657555187706899</v>
       </c>
     </row>
@@ -2952,16 +2959,16 @@
       <c r="B29" s="47">
         <v>0.145605920444033</v>
       </c>
-      <c r="C29" s="65">
-        <f t="shared" ref="C29:E29" si="23">C63*$F$44</f>
+      <c r="C29" s="61">
+        <f t="shared" ref="C29:E29" si="24">C63*$F$44</f>
         <v>-12.39380398905006</v>
       </c>
-      <c r="D29" s="65">
-        <f t="shared" si="23"/>
+      <c r="D29" s="61">
+        <f t="shared" si="24"/>
         <v>13.907909710630797</v>
       </c>
-      <c r="E29" s="65">
-        <f t="shared" si="23"/>
+      <c r="E29" s="61">
+        <f t="shared" si="24"/>
         <v>15.503102223112601</v>
       </c>
       <c r="G29" s="48" t="s">
@@ -2970,13 +2977,13 @@
       <c r="H29" s="47">
         <v>0.45753991832353902</v>
       </c>
-      <c r="I29" s="65">
+      <c r="I29" s="61">
         <v>-5.1696546894260398E-3</v>
       </c>
-      <c r="J29" s="65">
+      <c r="J29" s="61">
         <v>2.5456437079059979E-2</v>
       </c>
-      <c r="K29" s="65">
+      <c r="K29" s="61">
         <v>-4.0635182107980339E-3</v>
       </c>
       <c r="Y29" s="44" t="s">
@@ -3008,16 +3015,16 @@
       <c r="B30" s="47">
         <v>0.14363093014568501</v>
       </c>
-      <c r="C30" s="65">
-        <f t="shared" ref="C30:E30" si="24">C64*$F$44</f>
+      <c r="C30" s="61">
+        <f t="shared" ref="C30:E30" si="25">C64*$F$44</f>
         <v>-12.687624065378921</v>
       </c>
-      <c r="D30" s="65">
-        <f t="shared" si="24"/>
+      <c r="D30" s="61">
+        <f t="shared" si="25"/>
         <v>13.225054022190596</v>
       </c>
-      <c r="E30" s="65">
-        <f t="shared" si="24"/>
+      <c r="E30" s="61">
+        <f t="shared" si="25"/>
         <v>14.063118639089101</v>
       </c>
       <c r="G30" s="48" t="s">
@@ -3026,13 +3033,13 @@
       <c r="H30" s="47">
         <v>0.38030056637717502</v>
       </c>
-      <c r="I30" s="65">
+      <c r="I30" s="61">
         <v>-0.20093696667773603</v>
       </c>
-      <c r="J30" s="65">
+      <c r="J30" s="61">
         <v>6.4339879897847008E-2</v>
       </c>
-      <c r="K30" s="65">
+      <c r="K30" s="61">
         <v>6.9121556505988002E-2</v>
       </c>
       <c r="Y30" s="44" t="s">
@@ -3064,16 +3071,16 @@
       <c r="B31" s="47">
         <v>0.13989253288864101</v>
       </c>
-      <c r="C31" s="65">
-        <f t="shared" ref="C31:E31" si="25">C65*$F$44</f>
+      <c r="C31" s="61">
+        <f t="shared" ref="C31:E31" si="26">C65*$F$44</f>
         <v>-12.78895321384535</v>
       </c>
-      <c r="D31" s="65">
-        <f t="shared" si="25"/>
+      <c r="D31" s="61">
+        <f t="shared" si="26"/>
         <v>14.2558518597943</v>
       </c>
-      <c r="E31" s="65">
-        <f t="shared" si="25"/>
+      <c r="E31" s="61">
+        <f t="shared" si="26"/>
         <v>13.882617108779399</v>
       </c>
       <c r="G31" s="48" t="s">
@@ -3082,13 +3089,13 @@
       <c r="H31" s="47">
         <v>0.35071510667658901</v>
       </c>
-      <c r="I31" s="65">
+      <c r="I31" s="61">
         <v>-0.222364143018634</v>
       </c>
-      <c r="J31" s="65">
+      <c r="J31" s="61">
         <v>0.10034715691759399</v>
       </c>
-      <c r="K31" s="65">
+      <c r="K31" s="61">
         <v>9.624225669870401E-2</v>
       </c>
       <c r="Y31" s="44" t="s">
@@ -3123,16 +3130,16 @@
       <c r="B32" s="47">
         <v>7.9962894248608501E-2</v>
       </c>
-      <c r="C32" s="65">
-        <f t="shared" ref="C32:E32" si="26">C66*$F$44</f>
+      <c r="C32" s="61">
+        <f t="shared" ref="C32:E32" si="27">C66*$F$44</f>
         <v>-7.9962894248608505</v>
       </c>
-      <c r="D32" s="65">
-        <f t="shared" si="26"/>
+      <c r="D32" s="61">
+        <f t="shared" si="27"/>
         <v>19.12609205253715</v>
       </c>
-      <c r="E32" s="65">
-        <f t="shared" si="26"/>
+      <c r="E32" s="61">
+        <f t="shared" si="27"/>
         <v>61.697955179455654</v>
       </c>
       <c r="G32" s="48" t="s">
@@ -3141,13 +3148,13 @@
       <c r="H32" s="47">
         <v>0.38050271045420703</v>
       </c>
-      <c r="I32" s="65">
+      <c r="I32" s="61">
         <v>-0.20695715447495502</v>
       </c>
-      <c r="J32" s="65">
+      <c r="J32" s="61">
         <v>6.9257589485578974E-2</v>
       </c>
-      <c r="K32" s="65">
+      <c r="K32" s="61">
         <v>7.1860257501579983E-2</v>
       </c>
       <c r="Y32" s="44" t="s">
@@ -3179,16 +3186,16 @@
       <c r="B33" s="47">
         <v>4.6175788910679201E-2</v>
       </c>
-      <c r="C33" s="65">
-        <f t="shared" ref="C33:E33" si="27">C67*$F$44</f>
+      <c r="C33" s="61">
+        <f t="shared" ref="C33:E33" si="28">C67*$F$44</f>
         <v>-4.4666639693550367</v>
       </c>
-      <c r="D33" s="65">
-        <f t="shared" si="27"/>
+      <c r="D33" s="61">
+        <f t="shared" si="28"/>
         <v>13.507309282129382</v>
       </c>
-      <c r="E33" s="65">
-        <f t="shared" si="27"/>
+      <c r="E33" s="61">
+        <f t="shared" si="28"/>
         <v>14.23966827943218</v>
       </c>
       <c r="G33" s="48" t="s">
@@ -3197,13 +3204,13 @@
       <c r="H33" s="47">
         <v>0.36854947288399598</v>
       </c>
-      <c r="I33" s="65">
+      <c r="I33" s="61">
         <v>-0.23306069157825099</v>
       </c>
-      <c r="J33" s="65">
+      <c r="J33" s="61">
         <v>8.2205068342366017E-2</v>
       </c>
-      <c r="K33" s="65">
+      <c r="K33" s="61">
         <v>8.2195960833900017E-2</v>
       </c>
       <c r="Y33" s="44" t="s">
@@ -3235,16 +3242,16 @@
       <c r="B34" s="47">
         <v>9.3646713183988192E-3</v>
       </c>
-      <c r="C34" s="65">
-        <f t="shared" ref="C34:E34" si="28">C68*$F$44</f>
+      <c r="C34" s="61">
+        <f t="shared" ref="C34:E34" si="29">C68*$F$44</f>
         <v>-0.93646713183988195</v>
       </c>
-      <c r="D34" s="65">
-        <f t="shared" si="28"/>
+      <c r="D34" s="61">
+        <f t="shared" si="29"/>
         <v>63.562328495360418</v>
       </c>
-      <c r="E34" s="65">
-        <f t="shared" si="28"/>
+      <c r="E34" s="61">
+        <f t="shared" si="29"/>
         <v>97.534870447777919</v>
       </c>
       <c r="G34" s="48" t="s">
@@ -3253,13 +3260,13 @@
       <c r="H34" s="47">
         <v>0.380581779723702</v>
       </c>
-      <c r="I34" s="65">
+      <c r="I34" s="61">
         <v>-0.185851291382299</v>
       </c>
-      <c r="J34" s="65">
+      <c r="J34" s="61">
         <v>6.8216885120572002E-2</v>
       </c>
-      <c r="K34" s="65">
+      <c r="K34" s="61">
         <v>6.9887065377680024E-2</v>
       </c>
       <c r="Y34" s="48" t="s">
@@ -3291,16 +3298,16 @@
       <c r="B35" s="47">
         <v>0</v>
       </c>
-      <c r="C35" s="65">
-        <f t="shared" ref="C35:E35" si="29">C69*$F$44</f>
-        <v>0</v>
-      </c>
-      <c r="D35" s="65">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="E35" s="65">
-        <f t="shared" si="29"/>
+      <c r="C35" s="61">
+        <f t="shared" ref="C35:E35" si="30">C69*$F$44</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="61">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="61">
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="G35" s="48" t="s">
@@ -3309,128 +3316,128 @@
       <c r="H35" s="47">
         <v>0.37722451137045099</v>
       </c>
-      <c r="I35" s="65">
+      <c r="I35" s="61">
         <v>-0.23022733814822599</v>
       </c>
-      <c r="J35" s="65">
+      <c r="J35" s="61">
         <v>7.259609920082799E-2</v>
       </c>
-      <c r="K35" s="65">
+      <c r="K35" s="61">
         <v>7.6737779778277004E-2</v>
       </c>
-      <c r="Y35" s="61" t="s">
+      <c r="Y35" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="Z35" s="61"/>
-      <c r="AA35" s="61"/>
-      <c r="AB35" s="61"/>
+      <c r="Z35" s="64"/>
+      <c r="AA35" s="64"/>
+      <c r="AB35" s="64"/>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A36" s="61" t="s">
+      <c r="A36" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="61"/>
-      <c r="C36" s="61"/>
-      <c r="D36" s="61"/>
-      <c r="G36" s="61" t="s">
+      <c r="B36" s="64"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="64"/>
+      <c r="G36" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="H36" s="61"/>
-      <c r="I36" s="61"/>
-      <c r="J36" s="61"/>
-      <c r="Y36" s="62" t="s">
+      <c r="H36" s="64"/>
+      <c r="I36" s="64"/>
+      <c r="J36" s="64"/>
+      <c r="Y36" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="Z36" s="62"/>
-      <c r="AA36" s="62"/>
-      <c r="AB36" s="62"/>
+      <c r="Z36" s="63"/>
+      <c r="AA36" s="63"/>
+      <c r="AB36" s="63"/>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A37" s="62" t="s">
+      <c r="A37" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="62"/>
-      <c r="C37" s="62"/>
-      <c r="D37" s="62"/>
-      <c r="G37" s="62" t="s">
+      <c r="B37" s="63"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
+      <c r="G37" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="H37" s="62"/>
-      <c r="I37" s="62"/>
-      <c r="J37" s="62"/>
-      <c r="Y37" s="62" t="s">
+      <c r="H37" s="63"/>
+      <c r="I37" s="63"/>
+      <c r="J37" s="63"/>
+      <c r="Y37" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="Z37" s="62"/>
-      <c r="AA37" s="62"/>
-      <c r="AB37" s="62"/>
+      <c r="Z37" s="63"/>
+      <c r="AA37" s="63"/>
+      <c r="AB37" s="63"/>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A38" s="62" t="s">
+      <c r="A38" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="B38" s="62"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
-      <c r="G38" s="62" t="s">
+      <c r="B38" s="63"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
+      <c r="G38" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="H38" s="62"/>
-      <c r="I38" s="62"/>
-      <c r="J38" s="62"/>
+      <c r="H38" s="63"/>
+      <c r="I38" s="63"/>
+      <c r="J38" s="63"/>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C40" s="66">
+      <c r="C40" s="62">
         <v>-0.14245749712799199</v>
       </c>
-      <c r="D40" s="66">
+      <c r="D40" s="62">
         <v>0.13168131768538199</v>
       </c>
-      <c r="E40" s="66">
+      <c r="E40" s="62">
         <v>0.15056045822043101</v>
       </c>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C41" s="66">
+      <c r="C41" s="62">
         <v>-0.90577729178057231</v>
       </c>
-      <c r="D41" s="66">
-        <v>0</v>
-      </c>
-      <c r="E41" s="66">
+      <c r="D41" s="62">
+        <v>0</v>
+      </c>
+      <c r="E41" s="62">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C42" s="66">
+      <c r="C42" s="62">
         <v>-1.1345195611400016E-2</v>
       </c>
-      <c r="D42" s="66">
+      <c r="D42" s="62">
         <v>-8.9797671342489727E-3</v>
       </c>
-      <c r="E42" s="66">
+      <c r="E42" s="62">
         <v>7.2351713859910016E-2</v>
       </c>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C43" s="66">
+      <c r="C43" s="62">
         <v>-0.14252916143347749</v>
       </c>
-      <c r="D43" s="66">
+      <c r="D43" s="62">
         <v>7.6711958199159991E-2</v>
       </c>
-      <c r="E43" s="66">
+      <c r="E43" s="62">
         <v>8.9158559809736027E-2</v>
       </c>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C44" s="66">
+      <c r="C44" s="62">
         <v>-0.150286707891922</v>
       </c>
-      <c r="D44" s="66">
+      <c r="D44" s="62">
         <v>0.10012794231589001</v>
       </c>
-      <c r="E44" s="66">
+      <c r="E44" s="62">
         <v>8.9084524564714995E-2</v>
       </c>
       <c r="F44" s="42">
@@ -3438,277 +3445,277 @@
       </c>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C45" s="66">
+      <c r="C45" s="62">
         <v>-0.14776347763777289</v>
       </c>
-      <c r="D45" s="66">
+      <c r="D45" s="62">
         <v>0.10110985404686398</v>
       </c>
-      <c r="E45" s="66">
+      <c r="E45" s="62">
         <v>8.9728663937356984E-2</v>
       </c>
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C46" s="66">
+      <c r="C46" s="62">
         <v>-0.15067252683261609</v>
       </c>
-      <c r="D46" s="66">
+      <c r="D46" s="62">
         <v>9.8349148112096024E-2</v>
       </c>
-      <c r="E46" s="66">
+      <c r="E46" s="62">
         <v>9.8256913925116013E-2</v>
       </c>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C47" s="66">
+      <c r="C47" s="62">
         <v>-0.14331168329623573</v>
       </c>
-      <c r="D47" s="66">
+      <c r="D47" s="62">
         <v>0.10157634350679701</v>
       </c>
-      <c r="E47" s="66">
+      <c r="E47" s="62">
         <v>0.10857215987008101</v>
       </c>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C48" s="66">
+      <c r="C48" s="62">
         <v>-0.14895631065005391</v>
       </c>
-      <c r="D48" s="66">
+      <c r="D48" s="62">
         <v>0.10291024748335398</v>
       </c>
-      <c r="E48" s="66">
+      <c r="E48" s="62">
         <v>9.0820480981728013E-2</v>
       </c>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C49" s="66">
+      <c r="C49" s="62">
         <v>-0.14911703260337589</v>
       </c>
-      <c r="D49" s="66">
+      <c r="D49" s="62">
         <v>0.10693399483324098</v>
       </c>
-      <c r="E49" s="66">
+      <c r="E49" s="62">
         <v>0.10206807215909999</v>
       </c>
     </row>
     <row r="50" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C50" s="66">
+      <c r="C50" s="62">
         <v>-0.13624149824030349</v>
       </c>
-      <c r="D50" s="66">
+      <c r="D50" s="62">
         <v>0.10730574825316599</v>
       </c>
-      <c r="E50" s="66">
+      <c r="E50" s="62">
         <v>0.10387182215212001</v>
       </c>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C51" s="66">
+      <c r="C51" s="62">
         <v>-0.14454294685391941</v>
       </c>
-      <c r="D51" s="66">
+      <c r="D51" s="62">
         <v>0.11137570536473101</v>
       </c>
-      <c r="E51" s="66">
+      <c r="E51" s="62">
         <v>0.10593358617644699</v>
       </c>
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C52" s="66">
+      <c r="C52" s="62">
         <v>-0.142111488339728</v>
       </c>
-      <c r="D52" s="66">
+      <c r="D52" s="62">
         <v>0.10547562986648401</v>
       </c>
-      <c r="E52" s="66">
+      <c r="E52" s="62">
         <v>9.5929009684967981E-2</v>
       </c>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C53" s="66">
+      <c r="C53" s="62">
         <v>-0.14580901966684259</v>
       </c>
-      <c r="D53" s="66">
+      <c r="D53" s="62">
         <v>0.11942233401202498</v>
       </c>
-      <c r="E53" s="66">
+      <c r="E53" s="62">
         <v>0.11139984329844302</v>
       </c>
     </row>
     <row r="54" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C54" s="66">
+      <c r="C54" s="62">
         <v>-0.14607122766235481</v>
       </c>
-      <c r="D54" s="66">
+      <c r="D54" s="62">
         <v>0.11267911346254902</v>
       </c>
-      <c r="E54" s="66">
+      <c r="E54" s="62">
         <v>0.11346699225042803</v>
       </c>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C55" s="66">
+      <c r="C55" s="62">
         <v>-0.14787133544090639</v>
       </c>
-      <c r="D55" s="66">
+      <c r="D55" s="62">
         <v>0.10603543217919001</v>
       </c>
-      <c r="E55" s="66">
+      <c r="E55" s="62">
         <v>0.11055034414273499</v>
       </c>
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C56" s="66">
+      <c r="C56" s="62">
         <v>-0.1497242562906117</v>
       </c>
-      <c r="D56" s="66">
+      <c r="D56" s="62">
         <v>0.11861253596070803</v>
       </c>
-      <c r="E56" s="66">
+      <c r="E56" s="62">
         <v>0.10986437087608902</v>
       </c>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C57" s="66">
+      <c r="C57" s="62">
         <v>-0.14624630510994419</v>
       </c>
-      <c r="D57" s="66">
+      <c r="D57" s="62">
         <v>0.11644873835431102</v>
       </c>
-      <c r="E57" s="66">
+      <c r="E57" s="62">
         <v>0.106859486444908</v>
       </c>
     </row>
     <row r="58" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C58" s="66">
+      <c r="C58" s="62">
         <v>-0.13630487725860352</v>
       </c>
-      <c r="D58" s="66">
+      <c r="D58" s="62">
         <v>0.11955885509008501</v>
       </c>
-      <c r="E58" s="66">
+      <c r="E58" s="62">
         <v>0.11478419042311799</v>
       </c>
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C59" s="66">
+      <c r="C59" s="62">
         <v>-0.14487668456811301</v>
       </c>
-      <c r="D59" s="66">
+      <c r="D59" s="62">
         <v>0.12579854928525502</v>
       </c>
-      <c r="E59" s="66">
+      <c r="E59" s="62">
         <v>0.12529620608182201</v>
       </c>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C60" s="66">
+      <c r="C60" s="62">
         <v>-0.14340041416124111</v>
       </c>
-      <c r="D60" s="66">
+      <c r="D60" s="62">
         <v>0.12149335596483701</v>
       </c>
-      <c r="E60" s="66">
+      <c r="E60" s="62">
         <v>0.121512327346948</v>
       </c>
     </row>
     <row r="61" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C61" s="66">
+      <c r="C61" s="62">
         <v>-0.13541737959984451</v>
       </c>
-      <c r="D61" s="66">
+      <c r="D61" s="62">
         <v>0.13217976068322099</v>
       </c>
-      <c r="E61" s="66">
+      <c r="E61" s="62">
         <v>0.11601685113829099</v>
       </c>
     </row>
     <row r="62" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C62" s="66">
+      <c r="C62" s="62">
         <v>-0.14004970225573232</v>
       </c>
-      <c r="D62" s="66">
+      <c r="D62" s="62">
         <v>0.13833874155353698</v>
       </c>
-      <c r="E62" s="66">
+      <c r="E62" s="62">
         <v>0.13625011004124499</v>
       </c>
     </row>
     <row r="63" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C63" s="66">
+      <c r="C63" s="62">
         <v>-0.1239380398905006</v>
       </c>
-      <c r="D63" s="66">
+      <c r="D63" s="62">
         <v>0.13907909710630798</v>
       </c>
-      <c r="E63" s="66">
+      <c r="E63" s="62">
         <v>0.155031022231126</v>
       </c>
     </row>
     <row r="64" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C64" s="66">
+      <c r="C64" s="62">
         <v>-0.12687624065378922</v>
       </c>
-      <c r="D64" s="66">
+      <c r="D64" s="62">
         <v>0.13225054022190597</v>
       </c>
-      <c r="E64" s="66">
+      <c r="E64" s="62">
         <v>0.14063118639089101</v>
       </c>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C65" s="66">
+      <c r="C65" s="62">
         <v>-0.1278895321384535</v>
       </c>
-      <c r="D65" s="66">
+      <c r="D65" s="62">
         <v>0.142558518597943</v>
       </c>
-      <c r="E65" s="66">
+      <c r="E65" s="62">
         <v>0.13882617108779399</v>
       </c>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C66" s="66">
+      <c r="C66" s="62">
         <v>-7.9962894248608501E-2</v>
       </c>
-      <c r="D66" s="66">
+      <c r="D66" s="62">
         <v>0.1912609205253715</v>
       </c>
-      <c r="E66" s="66">
+      <c r="E66" s="62">
         <v>0.61697955179455655</v>
       </c>
     </row>
     <row r="67" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C67" s="66">
+      <c r="C67" s="62">
         <v>-4.4666639693550364E-2</v>
       </c>
-      <c r="D67" s="66">
+      <c r="D67" s="62">
         <v>0.13507309282129382</v>
       </c>
-      <c r="E67" s="66">
+      <c r="E67" s="62">
         <v>0.1423966827943218</v>
       </c>
     </row>
     <row r="68" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C68" s="66">
+      <c r="C68" s="62">
         <v>-9.3646713183988192E-3</v>
       </c>
-      <c r="D68" s="66">
+      <c r="D68" s="62">
         <v>0.63562328495360421</v>
       </c>
-      <c r="E68" s="66">
+      <c r="E68" s="62">
         <v>0.97534870447777922</v>
       </c>
     </row>
     <row r="69" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C69" s="66">
-        <v>0</v>
-      </c>
-      <c r="D69" s="66">
-        <v>0</v>
-      </c>
-      <c r="E69" s="66">
+      <c r="C69" s="62">
+        <v>0</v>
+      </c>
+      <c r="D69" s="62">
+        <v>0</v>
+      </c>
+      <c r="E69" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4265,8 +4272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T122"/>
   <sheetViews>
-    <sheetView topLeftCell="G28" workbookViewId="0">
-      <selection activeCell="T39" sqref="T39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9824,7 +9831,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10240,12 +10247,12 @@
       </c>
     </row>
     <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
       <c r="F17" s="3" t="s">
         <v>19</v>
       </c>
@@ -10260,12 +10267,12 @@
       </c>
     </row>
     <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="63" t="s">
+      <c r="A18" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="63"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
       <c r="F18" s="3" t="s">
         <v>20</v>
       </c>
@@ -10280,12 +10287,12 @@
       </c>
     </row>
     <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="63" t="s">
+      <c r="A19" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
       <c r="F19" s="3" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Created tables from the csvs within the ipynb file: both as csv (individually) and as latex (as a cell print)
</commit_message>
<xml_diff>
--- a/pre_processed_data/Analysis.xlsx
+++ b/pre_processed_data/Analysis.xlsx
@@ -581,6 +581,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -593,7 +594,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Incorreto" xfId="2" builtinId="27"/>
@@ -878,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AH8" sqref="AH8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -925,19 +925,19 @@
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="67" t="s">
+      <c r="G3" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="P3" s="42" t="s">
+      <c r="P3" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="Y3" s="42" t="s">
+      <c r="Y3" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="AH3" s="42" t="s">
+      <c r="AH3" s="63" t="s">
         <v>110</v>
       </c>
     </row>
@@ -3325,66 +3325,66 @@
       <c r="K35" s="61">
         <v>7.6737779778277004E-2</v>
       </c>
-      <c r="Y35" s="64" t="s">
+      <c r="Y35" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="Z35" s="64"/>
-      <c r="AA35" s="64"/>
-      <c r="AB35" s="64"/>
+      <c r="Z35" s="65"/>
+      <c r="AA35" s="65"/>
+      <c r="AB35" s="65"/>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A36" s="64" t="s">
+      <c r="A36" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="64"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="64"/>
-      <c r="G36" s="64" t="s">
+      <c r="B36" s="65"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
+      <c r="G36" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="H36" s="64"/>
-      <c r="I36" s="64"/>
-      <c r="J36" s="64"/>
-      <c r="Y36" s="63" t="s">
+      <c r="H36" s="65"/>
+      <c r="I36" s="65"/>
+      <c r="J36" s="65"/>
+      <c r="Y36" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="Z36" s="63"/>
-      <c r="AA36" s="63"/>
-      <c r="AB36" s="63"/>
+      <c r="Z36" s="64"/>
+      <c r="AA36" s="64"/>
+      <c r="AB36" s="64"/>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A37" s="63" t="s">
+      <c r="A37" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="63"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="63"/>
-      <c r="G37" s="63" t="s">
+      <c r="B37" s="64"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="64"/>
+      <c r="G37" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="H37" s="63"/>
-      <c r="I37" s="63"/>
-      <c r="J37" s="63"/>
-      <c r="Y37" s="63" t="s">
+      <c r="H37" s="64"/>
+      <c r="I37" s="64"/>
+      <c r="J37" s="64"/>
+      <c r="Y37" s="64" t="s">
         <v>65</v>
       </c>
-      <c r="Z37" s="63"/>
-      <c r="AA37" s="63"/>
-      <c r="AB37" s="63"/>
+      <c r="Z37" s="64"/>
+      <c r="AA37" s="64"/>
+      <c r="AB37" s="64"/>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A38" s="63" t="s">
+      <c r="A38" s="64" t="s">
         <v>65</v>
       </c>
-      <c r="B38" s="63"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="63"/>
-      <c r="G38" s="63" t="s">
+      <c r="B38" s="64"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="64"/>
+      <c r="G38" s="64" t="s">
         <v>65</v>
       </c>
-      <c r="H38" s="63"/>
-      <c r="I38" s="63"/>
-      <c r="J38" s="63"/>
+      <c r="H38" s="64"/>
+      <c r="I38" s="64"/>
+      <c r="J38" s="64"/>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="C40" s="62">
@@ -10247,12 +10247,12 @@
       </c>
     </row>
     <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="66"/>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
       <c r="F17" s="3" t="s">
         <v>19</v>
       </c>
@@ -10267,12 +10267,12 @@
       </c>
     </row>
     <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="65" t="s">
+      <c r="A18" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
       <c r="F18" s="3" t="s">
         <v>20</v>
       </c>
@@ -10287,12 +10287,12 @@
       </c>
     </row>
     <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="65" t="s">
+      <c r="A19" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="65"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
       <c r="F19" s="3" t="s">
         <v>21</v>
       </c>
@@ -13698,7 +13698,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>